<commit_message>
Update sheet contains information for generation icemr_variables.owl
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@72800 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="753" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="753" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Amazonia terms" sheetId="14" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="amazonia_censes" sheetId="7" r:id="rId6"/>
     <sheet name="data dictionary" sheetId="10" r:id="rId7"/>
     <sheet name="WebProtege" sheetId="12" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="15" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId9"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6941" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6815" uniqueCount="1312">
   <si>
     <t>Label</t>
   </si>
@@ -4061,7 +4061,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4835,7 +4835,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="PRISM terms"/>
@@ -5379,17 +5379,17 @@
       <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="35" t="s">
         <v>1091</v>
       </c>
@@ -7723,19 +7723,19 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="21" t="s">
         <v>754</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -8223,33 +8223,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Q81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="40" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="10" customWidth="1"/>
     <col min="6" max="6" width="19" style="10" customWidth="1"/>
-    <col min="7" max="8" width="19.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="33.1640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="34.33203125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="19.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="5" style="6" customWidth="1"/>
     <col min="12" max="12" width="18" style="6" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" style="8" customWidth="1"/>
     <col min="18" max="18" width="36" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="6"/>
+    <col min="20" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>468</v>
       </c>
@@ -12686,16 +12686,16 @@
       <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="34" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="36" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="18.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13574,17 +13574,17 @@
       <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="36" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16539,17 +16539,17 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="53.5" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18606,18 +18606,18 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="22.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -20317,7 +20317,7 @@
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
     </row>
-    <row r="50" spans="1:17" ht="28">
+    <row r="50" spans="1:17" ht="45">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -20339,7 +20339,7 @@
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" ht="30">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -21151,7 +21151,7 @@
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="1:17" ht="28">
+    <row r="80" spans="1:17" ht="45">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -21173,7 +21173,7 @@
       <c r="P80" s="6"/>
       <c r="Q80" s="6"/>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" ht="30">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
@@ -21989,7 +21989,7 @@
       <c r="P104" s="6"/>
       <c r="Q104" s="6"/>
     </row>
-    <row r="105" spans="1:17" ht="28">
+    <row r="105" spans="1:17" ht="30">
       <c r="A105" s="6" t="s">
         <v>215</v>
       </c>
@@ -22034,7 +22034,7 @@
       <c r="P105" s="6"/>
       <c r="Q105" s="6"/>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" ht="30">
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -22056,7 +22056,7 @@
       <c r="P106" s="6"/>
       <c r="Q106" s="6"/>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" ht="30">
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
@@ -23560,7 +23560,7 @@
       <c r="P164" s="6"/>
       <c r="Q164" s="6"/>
     </row>
-    <row r="165" spans="1:17" ht="28">
+    <row r="165" spans="1:17" ht="30">
       <c r="A165" s="6" t="s">
         <v>256</v>
       </c>
@@ -23764,7 +23764,7 @@
       <c r="P171" s="6"/>
       <c r="Q171" s="6"/>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="1:17" ht="30">
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
@@ -26715,11 +26715,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="52.1640625" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28564,15 +28564,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P174"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>469</v>
       </c>
@@ -28622,7 +28622,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15">
+    <row r="2" spans="1:16">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -28633,7 +28633,7 @@
       <c r="F2" s="6" t="s">
         <v>1070</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="6" t="s">
         <v>760</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -28660,7 +28660,9 @@
       <c r="O2" s="6" t="s">
         <v>744</v>
       </c>
-      <c r="P2" s="8"/>
+      <c r="P2" s="6" t="s">
+        <v>1311</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="32" t="s">
@@ -32406,585 +32408,25 @@
         <v>549</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>278</v>
+        <v>1069</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>1224</v>
       </c>
-      <c r="H81" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="I81" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J81" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K81" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="L81" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="M81" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N81" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O81" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="P81" s="8" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16">
-      <c r="A82" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="E82" s="32" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>1224</v>
-      </c>
-      <c r="H82" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="I82" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="J82" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K82" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="L82" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="M82" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="N82" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O82" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="P82" s="8" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16">
-      <c r="A83" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="E83" s="32" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>1224</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="J83" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K83" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="L83" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="M83" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N83" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O83" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="P83" s="8" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16">
-      <c r="A84" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="E84" s="32" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>1069</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>1224</v>
-      </c>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K84" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="P84" s="8"/>
-    </row>
-    <row r="96" spans="1:16">
-      <c r="C96" s="17" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3">
-      <c r="C97" s="17" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3">
-      <c r="C98" s="17" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3">
-      <c r="C99" s="6" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3">
-      <c r="C100" s="6" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3">
-      <c r="C101" s="6" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3">
-      <c r="C102" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="103" spans="3:3">
-      <c r="C103" s="17" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="104" spans="3:3">
-      <c r="C104" s="6" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="105" spans="3:3">
-      <c r="C105" s="6" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="106" spans="3:3">
-      <c r="C106" s="6" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="107" spans="3:3">
-      <c r="C107" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="108" spans="3:3">
-      <c r="C108" s="6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="109" spans="3:3">
-      <c r="C109" s="6" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="110" spans="3:3">
-      <c r="C110" s="6" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="111" spans="3:3">
-      <c r="C111" s="6" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="112" spans="3:3">
-      <c r="C112" s="6" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="113" spans="3:3">
-      <c r="C113" s="6" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="114" spans="3:3">
-      <c r="C114" s="17" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3">
-      <c r="C115" s="6" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="116" spans="3:3">
-      <c r="C116" s="6" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="117" spans="3:3">
-      <c r="C117" s="10" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="118" spans="3:3">
-      <c r="C118" s="32" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="119" spans="3:3">
-      <c r="C119" s="6" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="120" spans="3:3">
-      <c r="C120" s="32" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="121" spans="3:3">
-      <c r="C121" s="6" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="122" spans="3:3">
-      <c r="C122" s="6" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="123" spans="3:3">
-      <c r="C123" s="6" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="124" spans="3:3">
-      <c r="C124" s="6" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="125" spans="3:3">
-      <c r="C125" s="6" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="126" spans="3:3">
-      <c r="C126" s="6" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="127" spans="3:3">
-      <c r="C127" s="6" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="128" spans="3:3">
-      <c r="C128" s="6" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="129" spans="3:3">
-      <c r="C129" s="6" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3">
-      <c r="C130" s="6" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="131" spans="3:3">
-      <c r="C131" s="6" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="132" spans="3:3">
-      <c r="C132" s="6" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="133" spans="3:3">
-      <c r="C133" s="6" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="134" spans="3:3">
-      <c r="C134" s="6" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="135" spans="3:3">
-      <c r="C135" s="6" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="136" spans="3:3">
-      <c r="C136" s="6" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="137" spans="3:3">
-      <c r="C137" s="6" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="138" spans="3:3">
-      <c r="C138" s="6" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="139" spans="3:3">
-      <c r="C139" s="6" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="140" spans="3:3">
-      <c r="C140" s="6" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="141" spans="3:3">
-      <c r="C141" s="6" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="142" spans="3:3">
-      <c r="C142" s="6" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="143" spans="3:3">
-      <c r="C143" s="6" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="144" spans="3:3">
-      <c r="C144" s="6" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="145" spans="3:3">
-      <c r="C145" s="6" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="146" spans="3:3">
-      <c r="C146" s="6" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="147" spans="3:3">
-      <c r="C147" s="6" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="148" spans="3:3">
-      <c r="C148" s="6" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="149" spans="3:3">
-      <c r="C149" s="6" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="150" spans="3:3">
-      <c r="C150" s="6" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="151" spans="3:3">
-      <c r="C151" s="6" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="152" spans="3:3">
-      <c r="C152" s="6" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="153" spans="3:3">
-      <c r="C153" s="6" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="154" spans="3:3">
-      <c r="C154" s="6" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="155" spans="3:3">
-      <c r="C155" s="6" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="156" spans="3:3">
-      <c r="C156" s="6" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="157" spans="3:3">
-      <c r="C157" s="6" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="158" spans="3:3">
-      <c r="C158" s="6" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="159" spans="3:3">
-      <c r="C159" s="6" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="160" spans="3:3">
-      <c r="C160" s="6" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="161" spans="3:3">
-      <c r="C161" s="6" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="162" spans="3:3">
-      <c r="C162" s="6" t="s">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="163" spans="3:3">
-      <c r="C163" s="6" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="164" spans="3:3">
-      <c r="C164" s="6" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="165" spans="3:3">
-      <c r="C165" s="6" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="166" spans="3:3">
-      <c r="C166" s="6" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="167" spans="3:3">
-      <c r="C167" s="6" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="168" spans="3:3">
-      <c r="C168" s="6" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="169" spans="3:3">
-      <c r="C169" s="6" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="170" spans="3:3">
-      <c r="C170" s="17" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="171" spans="3:3">
-      <c r="C171" s="31" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="172" spans="3:3">
-      <c r="C172" s="6" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="173" spans="3:3">
-      <c r="C173" s="6" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="174" spans="3:3">
-      <c r="C174" s="6" t="s">
-        <v>1043</v>
-      </c>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="C96:C174">
-    <sortCondition ref="C96:C174"/>
-  </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move 'Sex' under 'Participant' for making it consistent as PRISM
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@74255 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="9440" windowWidth="29780" windowHeight="14180" tabRatio="753"/>
+    <workbookView xWindow="9495" yWindow="9435" windowWidth="29775" windowHeight="13740" tabRatio="753" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Amazonia terms" sheetId="14" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -6674,7 +6674,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7934,7 +7934,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="PRISM terms"/>
@@ -8474,21 +8474,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+    <sheetView topLeftCell="A123" workbookViewId="0">
       <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="33" t="s">
         <v>1073</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15">
+    <row r="103" spans="1:7" ht="15.75">
       <c r="A103" s="10" t="s">
         <v>2001</v>
       </c>
@@ -10849,7 +10849,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15">
+    <row r="104" spans="1:7" ht="15.75">
       <c r="A104" s="10" t="s">
         <v>2002</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15">
+    <row r="105" spans="1:7" ht="15.75">
       <c r="A105" s="18" t="s">
         <v>2003</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15">
+    <row r="106" spans="1:7" ht="15.75">
       <c r="A106" s="18" t="s">
         <v>2004</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15">
+    <row r="107" spans="1:7" ht="15.75">
       <c r="A107" s="10" t="s">
         <v>2005</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15">
+    <row r="108" spans="1:7" ht="15.75">
       <c r="A108" s="10" t="s">
         <v>2006</v>
       </c>
@@ -10964,7 +10964,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15">
+    <row r="109" spans="1:7" ht="15.75">
       <c r="A109" s="10" t="s">
         <v>2007</v>
       </c>
@@ -10987,7 +10987,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15">
+    <row r="110" spans="1:7" ht="15.75">
       <c r="A110" s="10" t="s">
         <v>2008</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15">
+    <row r="111" spans="1:7" ht="15.75">
       <c r="A111" s="10" t="s">
         <v>2009</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15">
+    <row r="112" spans="1:7" ht="15.75">
       <c r="A112" s="10" t="s">
         <v>2010</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15">
+    <row r="113" spans="1:7" ht="15.75">
       <c r="A113" s="10" t="s">
         <v>2011</v>
       </c>
@@ -11079,7 +11079,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15">
+    <row r="114" spans="1:7" ht="15.75">
       <c r="A114" s="10" t="s">
         <v>2012</v>
       </c>
@@ -11102,7 +11102,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15">
+    <row r="115" spans="1:7" ht="15.75">
       <c r="A115" s="10" t="s">
         <v>2013</v>
       </c>
@@ -11125,7 +11125,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15">
+    <row r="116" spans="1:7" ht="15.75">
       <c r="A116" s="10" t="s">
         <v>2014</v>
       </c>
@@ -11148,7 +11148,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15">
+    <row r="117" spans="1:7" ht="15.75">
       <c r="A117" s="10" t="s">
         <v>2015</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15">
+    <row r="118" spans="1:7" ht="15.75">
       <c r="A118" s="10" t="s">
         <v>2016</v>
       </c>
@@ -11194,7 +11194,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15">
+    <row r="119" spans="1:7" ht="15.75">
       <c r="A119" s="10" t="s">
         <v>2017</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15">
+    <row r="120" spans="1:7" ht="15.75">
       <c r="A120" s="10" t="s">
         <v>2018</v>
       </c>
@@ -11240,7 +11240,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15">
+    <row r="121" spans="1:7" ht="15.75">
       <c r="A121" s="10" t="s">
         <v>2019</v>
       </c>
@@ -11263,7 +11263,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15">
+    <row r="122" spans="1:7" ht="15.75">
       <c r="A122" s="10" t="s">
         <v>2020</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15">
+    <row r="123" spans="1:7" ht="15.75">
       <c r="A123" s="10" t="s">
         <v>2021</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15">
+    <row r="124" spans="1:7" ht="15.75">
       <c r="A124" s="10" t="s">
         <v>2022</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15">
+    <row r="125" spans="1:7" ht="15.75">
       <c r="A125" s="10" t="s">
         <v>2023</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15">
+    <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="10" t="s">
         <v>2024</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15">
+    <row r="127" spans="1:7" ht="15.75">
       <c r="A127" s="10" t="s">
         <v>2025</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15">
+    <row r="128" spans="1:7" ht="15.75">
       <c r="A128" s="10" t="s">
         <v>2026</v>
       </c>
@@ -11424,7 +11424,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15">
+    <row r="129" spans="1:7" ht="15.75">
       <c r="A129" s="10" t="s">
         <v>2027</v>
       </c>
@@ -11447,7 +11447,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15">
+    <row r="130" spans="1:7" ht="15.75">
       <c r="A130" s="10" t="s">
         <v>2028</v>
       </c>
@@ -11470,7 +11470,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15">
+    <row r="131" spans="1:7" ht="15.75">
       <c r="A131" s="10" t="s">
         <v>2029</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15">
+    <row r="132" spans="1:7" ht="15.75">
       <c r="A132" s="10" t="s">
         <v>2030</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15">
+    <row r="133" spans="1:7" ht="15.75">
       <c r="A133" s="10" t="s">
         <v>2031</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15">
+    <row r="134" spans="1:7" ht="15.75">
       <c r="A134" s="10" t="s">
         <v>2032</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15">
+    <row r="135" spans="1:7" ht="15.75">
       <c r="A135" s="10" t="s">
         <v>2033</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15">
+    <row r="136" spans="1:7" ht="15.75">
       <c r="A136" s="10" t="s">
         <v>2034</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15">
+    <row r="137" spans="1:7" ht="15.75">
       <c r="A137" s="10" t="s">
         <v>2035</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15">
+    <row r="138" spans="1:7" ht="15.75">
       <c r="A138" s="10" t="s">
         <v>2036</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15">
+    <row r="139" spans="1:7" ht="15.75">
       <c r="A139" s="10" t="s">
         <v>2037</v>
       </c>
@@ -11677,7 +11677,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15">
+    <row r="140" spans="1:7" ht="15.75">
       <c r="A140" s="10" t="s">
         <v>2038</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15">
+    <row r="141" spans="1:7" ht="15.75">
       <c r="A141" s="10" t="s">
         <v>2039</v>
       </c>
@@ -11723,7 +11723,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15">
+    <row r="142" spans="1:7" ht="15.75">
       <c r="A142" s="10" t="s">
         <v>2040</v>
       </c>
@@ -11746,7 +11746,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15">
+    <row r="143" spans="1:7" ht="15.75">
       <c r="A143" s="10" t="s">
         <v>2041</v>
       </c>
@@ -11769,7 +11769,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15">
+    <row r="144" spans="1:7" ht="15.75">
       <c r="A144" s="10" t="s">
         <v>2042</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15">
+    <row r="145" spans="1:7" ht="15.75">
       <c r="A145" s="10" t="s">
         <v>2043</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15">
+    <row r="146" spans="1:7" ht="15.75">
       <c r="A146" s="10" t="s">
         <v>2044</v>
       </c>
@@ -11838,7 +11838,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15">
+    <row r="147" spans="1:7" ht="15.75">
       <c r="A147" s="10" t="s">
         <v>2045</v>
       </c>
@@ -11861,7 +11861,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15">
+    <row r="148" spans="1:7" ht="15.75">
       <c r="A148" s="10" t="s">
         <v>2046</v>
       </c>
@@ -11884,7 +11884,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15">
+    <row r="149" spans="1:7" ht="15.75">
       <c r="A149" s="10" t="s">
         <v>2047</v>
       </c>
@@ -11907,7 +11907,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15">
+    <row r="150" spans="1:7" ht="15.75">
       <c r="A150" s="10" t="s">
         <v>2048</v>
       </c>
@@ -11930,7 +11930,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15">
+    <row r="151" spans="1:7" ht="15.75">
       <c r="A151" s="10" t="s">
         <v>2049</v>
       </c>
@@ -11953,7 +11953,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15">
+    <row r="152" spans="1:7" ht="15.75">
       <c r="A152" s="10" t="s">
         <v>2050</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15">
+    <row r="153" spans="1:7" ht="15.75">
       <c r="A153" s="10" t="s">
         <v>2051</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15">
+    <row r="154" spans="1:7" ht="15.75">
       <c r="A154" s="10" t="s">
         <v>2052</v>
       </c>
@@ -12022,7 +12022,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15">
+    <row r="155" spans="1:7" ht="15.75">
       <c r="A155" s="10" t="s">
         <v>2053</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15">
+    <row r="156" spans="1:7" ht="15.75">
       <c r="A156" s="10" t="s">
         <v>2054</v>
       </c>
@@ -12068,7 +12068,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15">
+    <row r="157" spans="1:7" ht="15.75">
       <c r="A157" s="10" t="s">
         <v>2055</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15">
+    <row r="158" spans="1:7" ht="15.75">
       <c r="A158" s="10" t="s">
         <v>2056</v>
       </c>
@@ -12114,7 +12114,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15">
+    <row r="159" spans="1:7" ht="15.75">
       <c r="A159" s="29" t="s">
         <v>2057</v>
       </c>
@@ -12137,7 +12137,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15">
+    <row r="160" spans="1:7" ht="15.75">
       <c r="A160" s="10" t="s">
         <v>2058</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15">
+    <row r="161" spans="1:7" ht="15.75">
       <c r="A161" s="10" t="s">
         <v>2059</v>
       </c>
@@ -12183,7 +12183,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15">
+    <row r="162" spans="1:7" ht="15.75">
       <c r="A162" s="10" t="s">
         <v>2060</v>
       </c>
@@ -12206,7 +12206,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15">
+    <row r="163" spans="1:7" ht="15.75">
       <c r="A163" s="18" t="s">
         <v>2061</v>
       </c>
@@ -12229,7 +12229,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15">
+    <row r="164" spans="1:7" ht="15.75">
       <c r="A164" s="10" t="s">
         <v>2062</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15">
+    <row r="165" spans="1:7" ht="15.75">
       <c r="A165" s="10" t="s">
         <v>2063</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15">
+    <row r="166" spans="1:7" ht="15.75">
       <c r="A166" s="10" t="s">
         <v>2064</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15">
+    <row r="167" spans="1:7" ht="15.75">
       <c r="A167" s="10" t="s">
         <v>2065</v>
       </c>
@@ -12321,7 +12321,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15">
+    <row r="168" spans="1:7" ht="15.75">
       <c r="A168" s="10" t="s">
         <v>2066</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15">
+    <row r="169" spans="1:7" ht="15.75">
       <c r="A169" s="10" t="s">
         <v>2067</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15">
+    <row r="170" spans="1:7" ht="15.75">
       <c r="A170" s="10" t="s">
         <v>2068</v>
       </c>
@@ -12390,7 +12390,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15">
+    <row r="171" spans="1:7" ht="15.75">
       <c r="A171" s="10" t="s">
         <v>2069</v>
       </c>
@@ -12413,7 +12413,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15">
+    <row r="172" spans="1:7" ht="15.75">
       <c r="A172" s="10" t="s">
         <v>2070</v>
       </c>
@@ -12436,7 +12436,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15">
+    <row r="173" spans="1:7" ht="15.75">
       <c r="A173" s="10" t="s">
         <v>2071</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15">
+    <row r="174" spans="1:7" ht="15.75">
       <c r="A174" s="10" t="s">
         <v>2072</v>
       </c>
@@ -12482,7 +12482,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15">
+    <row r="175" spans="1:7" ht="15.75">
       <c r="A175" s="10" t="s">
         <v>2073</v>
       </c>
@@ -12505,7 +12505,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15">
+    <row r="176" spans="1:7" ht="15.75">
       <c r="A176" s="10" t="s">
         <v>2074</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15">
+    <row r="177" spans="1:7" ht="15.75">
       <c r="A177" s="10" t="s">
         <v>2075</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15">
+    <row r="178" spans="1:7" ht="15.75">
       <c r="A178" s="10" t="s">
         <v>2076</v>
       </c>
@@ -12574,7 +12574,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15">
+    <row r="179" spans="1:7" ht="15.75">
       <c r="A179" s="10" t="s">
         <v>2077</v>
       </c>
@@ -12597,7 +12597,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15">
+    <row r="180" spans="1:7" ht="15.75">
       <c r="A180" s="10" t="s">
         <v>2078</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15">
+    <row r="181" spans="1:7" ht="15.75">
       <c r="A181" s="10" t="s">
         <v>2079</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15">
+    <row r="182" spans="1:7" ht="15.75">
       <c r="A182" s="10" t="s">
         <v>2080</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15">
+    <row r="183" spans="1:7" ht="15.75">
       <c r="A183" s="10" t="s">
         <v>2081</v>
       </c>
@@ -12689,7 +12689,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="15">
+    <row r="184" spans="1:7" ht="15.75">
       <c r="A184" s="10" t="s">
         <v>2082</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="15">
+    <row r="185" spans="1:7" ht="15.75">
       <c r="A185" s="10" t="s">
         <v>2083</v>
       </c>
@@ -12735,7 +12735,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="15">
+    <row r="186" spans="1:7" ht="15.75">
       <c r="A186" s="10" t="s">
         <v>2084</v>
       </c>
@@ -12758,7 +12758,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="15">
+    <row r="187" spans="1:7" ht="15.75">
       <c r="A187" s="10" t="s">
         <v>2085</v>
       </c>
@@ -12781,7 +12781,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15">
+    <row r="188" spans="1:7" ht="15.75">
       <c r="A188" s="10" t="s">
         <v>2086</v>
       </c>
@@ -12804,7 +12804,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="15">
+    <row r="189" spans="1:7" ht="15.75">
       <c r="A189" s="10" t="s">
         <v>2087</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="15">
+    <row r="190" spans="1:7" ht="15.75">
       <c r="A190" s="10" t="s">
         <v>2088</v>
       </c>
@@ -12850,7 +12850,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="15">
+    <row r="191" spans="1:7" ht="15.75">
       <c r="A191" s="17" t="s">
         <v>2089</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15">
+    <row r="192" spans="1:7" ht="15.75">
       <c r="A192" s="10" t="s">
         <v>2090</v>
       </c>
@@ -12896,7 +12896,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="15">
+    <row r="193" spans="1:7" ht="15.75">
       <c r="A193" s="10" t="s">
         <v>2091</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="15">
+    <row r="194" spans="1:7" ht="15.75">
       <c r="A194" s="10" t="s">
         <v>2092</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="15">
+    <row r="195" spans="1:7" ht="15.75">
       <c r="A195" s="10" t="s">
         <v>2093</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="15">
+    <row r="196" spans="1:7" ht="15.75">
       <c r="A196" s="10" t="s">
         <v>2094</v>
       </c>
@@ -12988,7 +12988,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15">
+    <row r="197" spans="1:7" ht="15.75">
       <c r="A197" s="10" t="s">
         <v>2095</v>
       </c>
@@ -13011,7 +13011,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15">
+    <row r="198" spans="1:7" ht="15.75">
       <c r="A198" s="10" t="s">
         <v>2096</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="15">
+    <row r="199" spans="1:7" ht="15.75">
       <c r="A199" s="10" t="s">
         <v>2097</v>
       </c>
@@ -13057,7 +13057,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="15">
+    <row r="200" spans="1:7" ht="15.75">
       <c r="A200" s="10" t="s">
         <v>2098</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="15">
+    <row r="201" spans="1:7" ht="15.75">
       <c r="A201" s="10" t="s">
         <v>2099</v>
       </c>
@@ -13103,7 +13103,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="15">
+    <row r="202" spans="1:7" ht="15.75">
       <c r="A202" s="10" t="s">
         <v>2100</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="15">
+    <row r="203" spans="1:7" ht="15.75">
       <c r="A203" s="10" t="s">
         <v>2101</v>
       </c>
@@ -13149,7 +13149,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="15">
+    <row r="204" spans="1:7" ht="15.75">
       <c r="A204" s="10" t="s">
         <v>2102</v>
       </c>
@@ -13172,7 +13172,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="15">
+    <row r="205" spans="1:7" ht="15.75">
       <c r="A205" s="10" t="s">
         <v>2103</v>
       </c>
@@ -13195,7 +13195,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="15">
+    <row r="206" spans="1:7" ht="15.75">
       <c r="A206" s="10" t="s">
         <v>2104</v>
       </c>
@@ -13218,7 +13218,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="15">
+    <row r="207" spans="1:7" ht="15.75">
       <c r="A207" s="10" t="s">
         <v>2105</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="15">
+    <row r="208" spans="1:7" ht="15.75">
       <c r="A208" s="10" t="s">
         <v>2106</v>
       </c>
@@ -13264,7 +13264,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="15">
+    <row r="209" spans="1:7" ht="15.75">
       <c r="A209" s="10" t="s">
         <v>2107</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="15">
+    <row r="210" spans="1:7" ht="15.75">
       <c r="A210" s="10" t="s">
         <v>2108</v>
       </c>
@@ -13310,7 +13310,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="15">
+    <row r="211" spans="1:7" ht="15.75">
       <c r="A211" s="10" t="s">
         <v>2109</v>
       </c>
@@ -13333,7 +13333,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="15">
+    <row r="212" spans="1:7" ht="15.75">
       <c r="A212" s="10" t="s">
         <v>2110</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="15">
+    <row r="213" spans="1:7" ht="15.75">
       <c r="A213" s="10" t="s">
         <v>2111</v>
       </c>
@@ -13379,7 +13379,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15">
+    <row r="214" spans="1:7" ht="15.75">
       <c r="A214" s="10" t="s">
         <v>2112</v>
       </c>
@@ -13402,7 +13402,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="15">
+    <row r="215" spans="1:7" ht="15.75">
       <c r="A215" s="10" t="s">
         <v>2113</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="15">
+    <row r="216" spans="1:7" ht="15.75">
       <c r="A216" s="10" t="s">
         <v>2114</v>
       </c>
@@ -13448,7 +13448,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="15">
+    <row r="217" spans="1:7" ht="15.75">
       <c r="A217" s="10" t="s">
         <v>2115</v>
       </c>
@@ -13471,7 +13471,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="15">
+    <row r="218" spans="1:7" ht="15.75">
       <c r="A218" s="10" t="s">
         <v>2116</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="15">
+    <row r="219" spans="1:7" ht="15.75">
       <c r="A219" s="10" t="s">
         <v>2117</v>
       </c>
@@ -13517,7 +13517,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="15">
+    <row r="220" spans="1:7" ht="15.75">
       <c r="A220" s="10" t="s">
         <v>2118</v>
       </c>
@@ -13540,7 +13540,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="15">
+    <row r="221" spans="1:7" ht="15.75">
       <c r="A221" s="10" t="s">
         <v>2119</v>
       </c>
@@ -13563,7 +13563,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="15">
+    <row r="222" spans="1:7" ht="15.75">
       <c r="A222" s="10" t="s">
         <v>2120</v>
       </c>
@@ -13586,7 +13586,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="15">
+    <row r="223" spans="1:7" ht="15.75">
       <c r="A223" s="10" t="s">
         <v>2121</v>
       </c>
@@ -13609,7 +13609,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="15">
+    <row r="224" spans="1:7" ht="15.75">
       <c r="A224" s="10" t="s">
         <v>2122</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="15">
+    <row r="225" spans="1:7" ht="15.75">
       <c r="A225" s="10" t="s">
         <v>2123</v>
       </c>
@@ -13655,7 +13655,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="15">
+    <row r="226" spans="1:7" ht="15.75">
       <c r="A226" s="10" t="s">
         <v>2124</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15">
+    <row r="227" spans="1:7" ht="15.75">
       <c r="A227" s="10" t="s">
         <v>2125</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="15">
+    <row r="228" spans="1:7" ht="15.75">
       <c r="A228" s="10" t="s">
         <v>2126</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="15">
+    <row r="229" spans="1:7" ht="15.75">
       <c r="A229" s="10" t="s">
         <v>2127</v>
       </c>
@@ -13747,7 +13747,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="15">
+    <row r="230" spans="1:7" ht="15.75">
       <c r="A230" s="10" t="s">
         <v>2128</v>
       </c>
@@ -13770,7 +13770,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="15">
+    <row r="231" spans="1:7" ht="15.75">
       <c r="A231" s="10" t="s">
         <v>2129</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="15">
+    <row r="232" spans="1:7" ht="15.75">
       <c r="A232" s="10" t="s">
         <v>2130</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="15">
+    <row r="233" spans="1:7" ht="15.75">
       <c r="A233" s="10" t="s">
         <v>2131</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="15">
+    <row r="234" spans="1:7" ht="15.75">
       <c r="A234" s="10" t="s">
         <v>2132</v>
       </c>
@@ -13862,7 +13862,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="15">
+    <row r="235" spans="1:7" ht="15.75">
       <c r="A235" s="10" t="s">
         <v>2133</v>
       </c>
@@ -13885,7 +13885,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="15">
+    <row r="236" spans="1:7" ht="15.75">
       <c r="A236" s="10" t="s">
         <v>2134</v>
       </c>
@@ -13908,7 +13908,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="15">
+    <row r="237" spans="1:7" ht="15.75">
       <c r="A237" s="10" t="s">
         <v>2135</v>
       </c>
@@ -13931,7 +13931,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="15">
+    <row r="238" spans="1:7" ht="15.75">
       <c r="A238" s="10" t="s">
         <v>2130</v>
       </c>
@@ -13954,7 +13954,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="15">
+    <row r="239" spans="1:7" ht="15.75">
       <c r="A239" s="10" t="s">
         <v>2136</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="15">
+    <row r="240" spans="1:7" ht="15.75">
       <c r="A240" s="10" t="s">
         <v>2137</v>
       </c>
@@ -14000,7 +14000,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="15">
+    <row r="241" spans="1:7" ht="15.75">
       <c r="A241" s="10" t="s">
         <v>2138</v>
       </c>
@@ -14023,7 +14023,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="15">
+    <row r="242" spans="1:7" ht="15.75">
       <c r="A242" s="10" t="s">
         <v>2139</v>
       </c>
@@ -14046,7 +14046,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="15">
+    <row r="243" spans="1:7" ht="15.75">
       <c r="A243" s="10" t="s">
         <v>2140</v>
       </c>
@@ -14069,7 +14069,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="15">
+    <row r="244" spans="1:7" ht="15.75">
       <c r="A244" s="10" t="s">
         <v>2141</v>
       </c>
@@ -14092,7 +14092,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="15">
+    <row r="245" spans="1:7" ht="15.75">
       <c r="A245" s="17" t="s">
         <v>2142</v>
       </c>
@@ -14115,7 +14115,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="15">
+    <row r="246" spans="1:7" ht="15.75">
       <c r="A246" s="10" t="s">
         <v>2143</v>
       </c>
@@ -14138,7 +14138,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="15">
+    <row r="247" spans="1:7" ht="15.75">
       <c r="A247" s="10" t="s">
         <v>2144</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="15">
+    <row r="248" spans="1:7" ht="15.75">
       <c r="A248" s="17" t="s">
         <v>2145</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="15">
+    <row r="249" spans="1:7" ht="15.75">
       <c r="A249" s="10" t="s">
         <v>2146</v>
       </c>
@@ -14207,7 +14207,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="15">
+    <row r="250" spans="1:7" ht="15.75">
       <c r="A250" s="10" t="s">
         <v>2147</v>
       </c>
@@ -14230,7 +14230,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="15">
+    <row r="251" spans="1:7" ht="15.75">
       <c r="A251" s="17" t="s">
         <v>2148</v>
       </c>
@@ -14253,7 +14253,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="15">
+    <row r="252" spans="1:7" ht="15.75">
       <c r="A252" s="10" t="s">
         <v>2149</v>
       </c>
@@ -14276,7 +14276,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="15">
+    <row r="253" spans="1:7" ht="15.75">
       <c r="A253" s="10" t="s">
         <v>2150</v>
       </c>
@@ -14299,7 +14299,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="15">
+    <row r="254" spans="1:7" ht="15.75">
       <c r="A254" s="10" t="s">
         <v>2151</v>
       </c>
@@ -14322,7 +14322,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="15">
+    <row r="255" spans="1:7" ht="15.75">
       <c r="A255" s="10" t="s">
         <v>2152</v>
       </c>
@@ -14345,7 +14345,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="15">
+    <row r="256" spans="1:7" ht="15.75">
       <c r="A256" s="10" t="s">
         <v>2153</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="15">
+    <row r="257" spans="1:7" ht="15.75">
       <c r="A257" s="10" t="s">
         <v>2154</v>
       </c>
@@ -14391,7 +14391,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="15">
+    <row r="258" spans="1:7" ht="15.75">
       <c r="A258" s="10" t="s">
         <v>2155</v>
       </c>
@@ -14414,7 +14414,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="15">
+    <row r="259" spans="1:7" ht="15.75">
       <c r="A259" s="17" t="s">
         <v>2156</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="15">
+    <row r="260" spans="1:7" ht="15.75">
       <c r="A260" s="10" t="s">
         <v>2157</v>
       </c>
@@ -14460,7 +14460,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="15">
+    <row r="261" spans="1:7" ht="15.75">
       <c r="A261" s="10" t="s">
         <v>2158</v>
       </c>
@@ -14483,7 +14483,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="15">
+    <row r="262" spans="1:7" ht="15.75">
       <c r="A262" s="10" t="s">
         <v>2159</v>
       </c>
@@ -14506,7 +14506,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="15">
+    <row r="263" spans="1:7" ht="15.75">
       <c r="A263" s="10" t="s">
         <v>2160</v>
       </c>
@@ -14529,7 +14529,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="15">
+    <row r="264" spans="1:7" ht="15.75">
       <c r="A264" s="10" t="s">
         <v>2161</v>
       </c>
@@ -14552,7 +14552,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="15">
+    <row r="265" spans="1:7" ht="15.75">
       <c r="A265" s="10" t="s">
         <v>2162</v>
       </c>
@@ -14575,7 +14575,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="15">
+    <row r="266" spans="1:7" ht="15.75">
       <c r="A266" s="10" t="s">
         <v>2163</v>
       </c>
@@ -14598,7 +14598,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="15">
+    <row r="267" spans="1:7" ht="15.75">
       <c r="A267" s="10" t="s">
         <v>2164</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="15">
+    <row r="268" spans="1:7" ht="15.75">
       <c r="A268" s="10" t="s">
         <v>2165</v>
       </c>
@@ -14644,7 +14644,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="15">
+    <row r="269" spans="1:7" ht="15.75">
       <c r="A269" s="10" t="s">
         <v>2166</v>
       </c>
@@ -14667,7 +14667,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="15">
+    <row r="270" spans="1:7" ht="15.75">
       <c r="A270" s="10" t="s">
         <v>2167</v>
       </c>
@@ -14690,7 +14690,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="15">
+    <row r="271" spans="1:7" ht="15.75">
       <c r="A271" s="10" t="s">
         <v>2168</v>
       </c>
@@ -14713,7 +14713,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="15">
+    <row r="272" spans="1:7" ht="15.75">
       <c r="A272" s="10" t="s">
         <v>2169</v>
       </c>
@@ -14736,7 +14736,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="273" spans="1:7" ht="15">
+    <row r="273" spans="1:7" ht="15.75">
       <c r="A273" s="10" t="s">
         <v>2170</v>
       </c>
@@ -14759,7 +14759,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="15">
+    <row r="274" spans="1:7" ht="15.75">
       <c r="A274" s="10" t="s">
         <v>2171</v>
       </c>
@@ -14782,7 +14782,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="275" spans="1:7" ht="15">
+    <row r="275" spans="1:7" ht="15.75">
       <c r="A275" s="10" t="s">
         <v>2172</v>
       </c>
@@ -14805,7 +14805,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="276" spans="1:7" ht="15">
+    <row r="276" spans="1:7" ht="15.75">
       <c r="A276" s="10" t="s">
         <v>2173</v>
       </c>
@@ -14828,7 +14828,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="277" spans="1:7" ht="15">
+    <row r="277" spans="1:7" ht="15.75">
       <c r="A277" s="10" t="s">
         <v>2174</v>
       </c>
@@ -14851,7 +14851,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="278" spans="1:7" ht="15">
+    <row r="278" spans="1:7" ht="15.75">
       <c r="A278" s="10" t="s">
         <v>2175</v>
       </c>
@@ -14874,7 +14874,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="279" spans="1:7" ht="15">
+    <row r="279" spans="1:7" ht="15.75">
       <c r="A279" s="10" t="s">
         <v>2176</v>
       </c>
@@ -14897,7 +14897,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="280" spans="1:7" ht="15">
+    <row r="280" spans="1:7" ht="15.75">
       <c r="A280" s="18" t="s">
         <v>2178</v>
       </c>
@@ -14920,7 +14920,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="281" spans="1:7" ht="15">
+    <row r="281" spans="1:7" ht="15.75">
       <c r="A281" s="17" t="s">
         <v>2179</v>
       </c>
@@ -14962,20 +14962,20 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="21" t="s">
         <v>742</v>
       </c>
@@ -15004,7 +15004,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10" ht="15.75">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -15523,35 +15523,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:H54"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="10" customWidth="1"/>
     <col min="6" max="6" width="19" style="10" customWidth="1"/>
-    <col min="7" max="8" width="19.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="19.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="6" customWidth="1"/>
     <col min="12" max="12" width="18" style="6" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" style="8" customWidth="1"/>
     <col min="18" max="18" width="36" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="6"/>
+    <col min="20" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>466</v>
       </c>
@@ -17620,10 +17620,10 @@
         <v>3</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>540</v>
+        <v>561</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>541</v>
+        <v>562</v>
       </c>
       <c r="F42" s="30" t="s">
         <v>1163</v>
@@ -20108,21 +20108,21 @@
       <selection pane="bottomLeft" activeCell="A72" sqref="A72:XFD72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="6" style="6" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="45.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" style="6" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="6"/>
+    <col min="10" max="10" width="27.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="42" customFormat="1" ht="38.25" customHeight="1">
@@ -20163,7 +20163,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="37" customFormat="1" ht="15">
+    <row r="2" spans="1:13" s="37" customFormat="1" ht="15.75">
       <c r="G2" s="10" t="s">
         <v>985</v>
       </c>
@@ -20183,7 +20183,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -20220,7 +20220,7 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="15">
+    <row r="4" spans="1:13" ht="15.75">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -20257,7 +20257,7 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="15">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -20294,7 +20294,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15">
+    <row r="6" spans="1:13" ht="15.75">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -20331,7 +20331,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="15">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -20368,7 +20368,7 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="15">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -20405,7 +20405,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="15">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -20442,7 +20442,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="15">
+    <row r="10" spans="1:13" ht="15.75">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -20479,7 +20479,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="15">
+    <row r="11" spans="1:13" ht="15.75">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -20516,7 +20516,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="15">
+    <row r="12" spans="1:13" ht="15.75">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -20553,7 +20553,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13" ht="15.75">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -20590,7 +20590,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="15">
+    <row r="14" spans="1:13" ht="15.75">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -20627,7 +20627,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="15">
+    <row r="15" spans="1:13" ht="15.75">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -20664,7 +20664,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="15.75">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -20701,7 +20701,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="15">
+    <row r="17" spans="1:13" ht="15.75">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -20738,7 +20738,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13" ht="15.75">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -20775,7 +20775,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="15">
+    <row r="19" spans="1:13" ht="15.75">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -20812,7 +20812,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="15">
+    <row r="20" spans="1:13" ht="15.75">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -20849,7 +20849,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="15">
+    <row r="21" spans="1:13" ht="15.75">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -20886,7 +20886,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="15">
+    <row r="22" spans="1:13" ht="15.75">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -20923,7 +20923,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="15">
+    <row r="23" spans="1:13" ht="15.75">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -20960,7 +20960,7 @@
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="15">
+    <row r="24" spans="1:13" ht="15.75">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -21034,7 +21034,7 @@
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="15">
+    <row r="26" spans="1:13" ht="15.75">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -21071,7 +21071,7 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" ht="15">
+    <row r="27" spans="1:13" ht="15.75">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -21145,7 +21145,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="15">
+    <row r="29" spans="1:13" ht="15.75">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -21182,7 +21182,7 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" ht="15">
+    <row r="30" spans="1:13" ht="15.75">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -21219,7 +21219,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15">
+    <row r="31" spans="1:13" ht="15.75">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -21256,7 +21256,7 @@
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="15">
+    <row r="32" spans="1:13" ht="15.75">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -21293,7 +21293,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="1:13" ht="15">
+    <row r="33" spans="1:13" ht="15.75">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -21330,7 +21330,7 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" ht="15">
+    <row r="34" spans="1:13" ht="15.75">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -21367,7 +21367,7 @@
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="1:13" ht="15">
+    <row r="35" spans="1:13" ht="15.75">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -21404,7 +21404,7 @@
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="1:13" ht="15">
+    <row r="36" spans="1:13" ht="15.75">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -21441,7 +21441,7 @@
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="1:13" ht="15">
+    <row r="37" spans="1:13" ht="15.75">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -21478,7 +21478,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="1:13" ht="15">
+    <row r="38" spans="1:13" ht="15.75">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -21515,7 +21515,7 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="1:13" ht="15">
+    <row r="39" spans="1:13" ht="15.75">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -21552,7 +21552,7 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="1:13" ht="15">
+    <row r="40" spans="1:13" ht="15.75">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -21589,7 +21589,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13" ht="15">
+    <row r="41" spans="1:13" ht="15.75">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -21626,7 +21626,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
     </row>
-    <row r="42" spans="1:13" ht="15">
+    <row r="42" spans="1:13" ht="15.75">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -21663,7 +21663,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" spans="1:13" ht="15">
+    <row r="43" spans="1:13" ht="15.75">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -21700,7 +21700,7 @@
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
     </row>
-    <row r="44" spans="1:13" ht="15">
+    <row r="44" spans="1:13" ht="15.75">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -21737,7 +21737,7 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" spans="1:13" ht="15">
+    <row r="45" spans="1:13" ht="15.75">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -21811,7 +21811,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="15">
+    <row r="47" spans="1:13" ht="15.75">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -21848,7 +21848,7 @@
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="15">
+    <row r="48" spans="1:13" ht="15.75">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -21885,7 +21885,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
     </row>
-    <row r="49" spans="1:13" ht="15">
+    <row r="49" spans="1:13" ht="15.75">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -21922,7 +21922,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
     </row>
-    <row r="50" spans="1:13" ht="15">
+    <row r="50" spans="1:13" ht="15.75">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -21959,7 +21959,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
     </row>
-    <row r="51" spans="1:13" ht="15">
+    <row r="51" spans="1:13" ht="15.75">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -21996,7 +21996,7 @@
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
     </row>
-    <row r="52" spans="1:13" ht="15">
+    <row r="52" spans="1:13" ht="15.75">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -22033,7 +22033,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:13" ht="15">
+    <row r="53" spans="1:13" ht="15.75">
       <c r="A53" s="10">
         <v>51</v>
       </c>
@@ -22070,7 +22070,7 @@
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="1:13" ht="15">
+    <row r="54" spans="1:13" ht="15.75">
       <c r="A54" s="10">
         <v>52</v>
       </c>
@@ -22107,7 +22107,7 @@
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
     </row>
-    <row r="55" spans="1:13" ht="15">
+    <row r="55" spans="1:13" ht="15.75">
       <c r="A55" s="10">
         <v>53</v>
       </c>
@@ -22144,7 +22144,7 @@
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
     </row>
-    <row r="56" spans="1:13" ht="15">
+    <row r="56" spans="1:13" ht="15.75">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -22255,7 +22255,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" ht="15">
+    <row r="59" spans="1:13" ht="15.75">
       <c r="A59" s="10">
         <v>57</v>
       </c>
@@ -22292,7 +22292,7 @@
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
     </row>
-    <row r="60" spans="1:13" ht="15">
+    <row r="60" spans="1:13" ht="15.75">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -22329,7 +22329,7 @@
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
     </row>
-    <row r="61" spans="1:13" ht="15">
+    <row r="61" spans="1:13" ht="15.75">
       <c r="A61" s="10">
         <v>59</v>
       </c>
@@ -22366,7 +22366,7 @@
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
     </row>
-    <row r="62" spans="1:13" ht="15">
+    <row r="62" spans="1:13" ht="15.75">
       <c r="A62" s="10">
         <v>60</v>
       </c>
@@ -22403,7 +22403,7 @@
       <c r="L62" s="10"/>
       <c r="M62" s="10"/>
     </row>
-    <row r="63" spans="1:13" ht="15">
+    <row r="63" spans="1:13" ht="15.75">
       <c r="A63" s="10">
         <v>61</v>
       </c>
@@ -22440,7 +22440,7 @@
       <c r="L63" s="10"/>
       <c r="M63" s="10"/>
     </row>
-    <row r="64" spans="1:13" ht="15">
+    <row r="64" spans="1:13" ht="15.75">
       <c r="A64" s="10">
         <v>62</v>
       </c>
@@ -22479,7 +22479,7 @@
       </c>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="1:13" ht="15">
+    <row r="65" spans="1:13" ht="15.75">
       <c r="A65" s="10">
         <v>63</v>
       </c>
@@ -22518,7 +22518,7 @@
       </c>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="1:13" ht="15">
+    <row r="66" spans="1:13" ht="15.75">
       <c r="A66" s="10">
         <v>64</v>
       </c>
@@ -22555,7 +22555,7 @@
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="1:13" ht="15">
+    <row r="67" spans="1:13" ht="15.75">
       <c r="A67" s="10">
         <v>65</v>
       </c>
@@ -22592,7 +22592,7 @@
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
     </row>
-    <row r="68" spans="1:13" ht="15">
+    <row r="68" spans="1:13" ht="15.75">
       <c r="A68" s="10">
         <v>66</v>
       </c>
@@ -22629,7 +22629,7 @@
       <c r="L68" s="10"/>
       <c r="M68" s="10"/>
     </row>
-    <row r="69" spans="1:13" ht="15">
+    <row r="69" spans="1:13" ht="15.75">
       <c r="A69" s="10">
         <v>67</v>
       </c>
@@ -22666,7 +22666,7 @@
       <c r="L69" s="10"/>
       <c r="M69" s="10"/>
     </row>
-    <row r="70" spans="1:13" ht="15">
+    <row r="70" spans="1:13" ht="15.75">
       <c r="A70" s="10">
         <v>68</v>
       </c>
@@ -22703,7 +22703,7 @@
       <c r="L70" s="10"/>
       <c r="M70" s="10"/>
     </row>
-    <row r="71" spans="1:13" ht="15">
+    <row r="71" spans="1:13" ht="15.75">
       <c r="A71" s="10">
         <v>69</v>
       </c>
@@ -22740,7 +22740,7 @@
       <c r="L71" s="10"/>
       <c r="M71" s="10"/>
     </row>
-    <row r="72" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="72" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A72" s="10">
         <v>70</v>
       </c>
@@ -22777,7 +22777,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:13" ht="15">
+    <row r="73" spans="1:13" ht="15.75">
       <c r="A73" s="10">
         <v>71</v>
       </c>
@@ -22816,7 +22816,7 @@
       </c>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="1:13" ht="15">
+    <row r="74" spans="1:13" ht="15.75">
       <c r="A74" s="10">
         <v>72</v>
       </c>
@@ -22855,7 +22855,7 @@
       </c>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="1:13" ht="15">
+    <row r="75" spans="1:13" ht="15.75">
       <c r="A75" s="10">
         <v>73</v>
       </c>
@@ -22894,7 +22894,7 @@
       </c>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="1:13" ht="15">
+    <row r="76" spans="1:13" ht="15.75">
       <c r="A76" s="10">
         <v>74</v>
       </c>
@@ -22931,7 +22931,7 @@
       <c r="L76" s="10"/>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="1:13" ht="15">
+    <row r="77" spans="1:13" ht="15.75">
       <c r="A77" s="10">
         <v>75</v>
       </c>
@@ -22968,7 +22968,7 @@
       <c r="L77" s="10"/>
       <c r="M77" s="10"/>
     </row>
-    <row r="78" spans="1:13" ht="15">
+    <row r="78" spans="1:13" ht="15.75">
       <c r="A78" s="10">
         <v>76</v>
       </c>
@@ -23005,7 +23005,7 @@
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:13" ht="15">
+    <row r="79" spans="1:13" ht="15.75">
       <c r="A79" s="10">
         <v>77</v>
       </c>
@@ -23042,7 +23042,7 @@
       <c r="L79" s="10"/>
       <c r="M79" s="10"/>
     </row>
-    <row r="80" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="80" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A80" s="10">
         <v>78</v>
       </c>
@@ -23079,7 +23079,7 @@
       <c r="L80" s="10"/>
       <c r="M80" s="10"/>
     </row>
-    <row r="81" spans="1:13" ht="15">
+    <row r="81" spans="1:13" ht="15.75">
       <c r="A81" s="10">
         <v>79</v>
       </c>
@@ -23116,7 +23116,7 @@
       <c r="L81" s="10"/>
       <c r="M81" s="10"/>
     </row>
-    <row r="82" spans="1:13" ht="15">
+    <row r="82" spans="1:13" ht="15.75">
       <c r="A82" s="10">
         <v>80</v>
       </c>
@@ -23153,7 +23153,7 @@
       <c r="L82" s="10"/>
       <c r="M82" s="10"/>
     </row>
-    <row r="83" spans="1:13" ht="15">
+    <row r="83" spans="1:13" ht="15.75">
       <c r="A83" s="10">
         <v>81</v>
       </c>
@@ -23190,7 +23190,7 @@
       <c r="L83" s="10"/>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="1:13" ht="15">
+    <row r="84" spans="1:13" ht="15.75">
       <c r="A84" s="10">
         <v>82</v>
       </c>
@@ -23227,7 +23227,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" ht="15">
+    <row r="85" spans="1:13" ht="15.75">
       <c r="A85" s="10">
         <v>83</v>
       </c>
@@ -23264,7 +23264,7 @@
       <c r="L85" s="10"/>
       <c r="M85" s="10"/>
     </row>
-    <row r="86" spans="1:13" ht="15">
+    <row r="86" spans="1:13" ht="15.75">
       <c r="A86" s="10">
         <v>84</v>
       </c>
@@ -23301,7 +23301,7 @@
       <c r="L86" s="10"/>
       <c r="M86" s="10"/>
     </row>
-    <row r="87" spans="1:13" ht="15">
+    <row r="87" spans="1:13" ht="15.75">
       <c r="A87" s="10">
         <v>85</v>
       </c>
@@ -23340,7 +23340,7 @@
       </c>
       <c r="M87" s="10"/>
     </row>
-    <row r="88" spans="1:13" ht="15">
+    <row r="88" spans="1:13" ht="15.75">
       <c r="A88" s="10">
         <v>86</v>
       </c>
@@ -23379,7 +23379,7 @@
       </c>
       <c r="M88" s="10"/>
     </row>
-    <row r="89" spans="1:13" ht="15">
+    <row r="89" spans="1:13" ht="15.75">
       <c r="A89" s="10">
         <v>87</v>
       </c>
@@ -23418,7 +23418,7 @@
       </c>
       <c r="M89" s="10"/>
     </row>
-    <row r="90" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="90" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A90" s="10">
         <v>88</v>
       </c>
@@ -23455,7 +23455,7 @@
       <c r="L90" s="10"/>
       <c r="M90" s="10"/>
     </row>
-    <row r="91" spans="1:13" ht="15">
+    <row r="91" spans="1:13" ht="15.75">
       <c r="A91" s="10">
         <v>89</v>
       </c>
@@ -23492,7 +23492,7 @@
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
     </row>
-    <row r="92" spans="1:13" ht="15">
+    <row r="92" spans="1:13" ht="15.75">
       <c r="A92" s="10">
         <v>90</v>
       </c>
@@ -23529,7 +23529,7 @@
       <c r="L92" s="10"/>
       <c r="M92" s="10"/>
     </row>
-    <row r="93" spans="1:13" ht="15">
+    <row r="93" spans="1:13" ht="15.75">
       <c r="A93" s="10">
         <v>91</v>
       </c>
@@ -23566,7 +23566,7 @@
       <c r="L93" s="10"/>
       <c r="M93" s="10"/>
     </row>
-    <row r="94" spans="1:13" ht="15">
+    <row r="94" spans="1:13" ht="15.75">
       <c r="A94" s="10">
         <v>92</v>
       </c>
@@ -23603,7 +23603,7 @@
       <c r="L94" s="10"/>
       <c r="M94" s="10"/>
     </row>
-    <row r="95" spans="1:13" ht="15">
+    <row r="95" spans="1:13" ht="15.75">
       <c r="A95" s="10">
         <v>93</v>
       </c>
@@ -23640,7 +23640,7 @@
       <c r="L95" s="10"/>
       <c r="M95" s="10"/>
     </row>
-    <row r="96" spans="1:13" ht="15">
+    <row r="96" spans="1:13" ht="15.75">
       <c r="A96" s="10">
         <v>94</v>
       </c>
@@ -23677,7 +23677,7 @@
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
     </row>
-    <row r="97" spans="1:13" ht="15">
+    <row r="97" spans="1:13" ht="15.75">
       <c r="A97" s="10">
         <v>95</v>
       </c>
@@ -23716,7 +23716,7 @@
       </c>
       <c r="M97" s="10"/>
     </row>
-    <row r="98" spans="1:13" ht="15">
+    <row r="98" spans="1:13" ht="15.75">
       <c r="A98" s="10">
         <v>96</v>
       </c>
@@ -23753,7 +23753,7 @@
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
     </row>
-    <row r="99" spans="1:13" ht="15">
+    <row r="99" spans="1:13" ht="15.75">
       <c r="A99" s="10">
         <v>97</v>
       </c>
@@ -23790,7 +23790,7 @@
       <c r="L99" s="10"/>
       <c r="M99" s="10"/>
     </row>
-    <row r="100" spans="1:13" ht="15">
+    <row r="100" spans="1:13" ht="15.75">
       <c r="A100" s="10">
         <v>98</v>
       </c>
@@ -23829,7 +23829,7 @@
       </c>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="1:13" ht="15">
+    <row r="101" spans="1:13" ht="15.75">
       <c r="A101" s="10">
         <v>99</v>
       </c>
@@ -23866,7 +23866,7 @@
       <c r="L101" s="10"/>
       <c r="M101" s="10"/>
     </row>
-    <row r="102" spans="1:13" ht="15">
+    <row r="102" spans="1:13" ht="15.75">
       <c r="A102" s="10">
         <v>100</v>
       </c>
@@ -23905,7 +23905,7 @@
       </c>
       <c r="M102" s="10"/>
     </row>
-    <row r="103" spans="1:13" ht="15">
+    <row r="103" spans="1:13" ht="15.75">
       <c r="A103" s="10">
         <v>101</v>
       </c>
@@ -23942,7 +23942,7 @@
       <c r="L103" s="10"/>
       <c r="M103" s="10"/>
     </row>
-    <row r="104" spans="1:13" ht="15">
+    <row r="104" spans="1:13" ht="15.75">
       <c r="A104" s="10">
         <v>102</v>
       </c>
@@ -23979,7 +23979,7 @@
       <c r="L104" s="10"/>
       <c r="M104" s="10"/>
     </row>
-    <row r="105" spans="1:13" ht="15">
+    <row r="105" spans="1:13" ht="15.75">
       <c r="A105" s="10">
         <v>103</v>
       </c>
@@ -24016,7 +24016,7 @@
       <c r="L105" s="10"/>
       <c r="M105" s="10"/>
     </row>
-    <row r="106" spans="1:13" ht="15">
+    <row r="106" spans="1:13" ht="15.75">
       <c r="A106" s="10">
         <v>104</v>
       </c>
@@ -24053,7 +24053,7 @@
       <c r="L106" s="10"/>
       <c r="M106" s="10"/>
     </row>
-    <row r="107" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="107" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A107" s="10">
         <v>105</v>
       </c>
@@ -24090,7 +24090,7 @@
       <c r="L107" s="10"/>
       <c r="M107" s="10"/>
     </row>
-    <row r="108" spans="1:13" ht="15">
+    <row r="108" spans="1:13" ht="15.75">
       <c r="A108" s="10">
         <v>106</v>
       </c>
@@ -24127,7 +24127,7 @@
       <c r="L108" s="10"/>
       <c r="M108" s="10"/>
     </row>
-    <row r="109" spans="1:13" ht="15">
+    <row r="109" spans="1:13" ht="15.75">
       <c r="A109" s="10">
         <v>107</v>
       </c>
@@ -24164,7 +24164,7 @@
       <c r="L109" s="10"/>
       <c r="M109" s="10"/>
     </row>
-    <row r="110" spans="1:13" ht="15">
+    <row r="110" spans="1:13" ht="15.75">
       <c r="A110" s="10">
         <v>108</v>
       </c>
@@ -24201,7 +24201,7 @@
       <c r="L110" s="10"/>
       <c r="M110" s="10"/>
     </row>
-    <row r="111" spans="1:13" ht="15">
+    <row r="111" spans="1:13" ht="15.75">
       <c r="A111" s="10">
         <v>109</v>
       </c>
@@ -24238,7 +24238,7 @@
       <c r="L111" s="10"/>
       <c r="M111" s="10"/>
     </row>
-    <row r="112" spans="1:13" ht="15">
+    <row r="112" spans="1:13" ht="15.75">
       <c r="A112" s="10">
         <v>110</v>
       </c>
@@ -24275,7 +24275,7 @@
       <c r="L112" s="10"/>
       <c r="M112" s="10"/>
     </row>
-    <row r="113" spans="1:13" ht="15">
+    <row r="113" spans="1:13" ht="15.75">
       <c r="A113" s="10">
         <v>111</v>
       </c>
@@ -24312,7 +24312,7 @@
       <c r="L113" s="10"/>
       <c r="M113" s="10"/>
     </row>
-    <row r="114" spans="1:13" ht="15">
+    <row r="114" spans="1:13" ht="15.75">
       <c r="A114" s="10">
         <v>112</v>
       </c>
@@ -24386,7 +24386,7 @@
       <c r="L115" s="10"/>
       <c r="M115" s="10"/>
     </row>
-    <row r="116" spans="1:13" ht="15">
+    <row r="116" spans="1:13" ht="15.75">
       <c r="A116" s="10">
         <v>114</v>
       </c>
@@ -24423,7 +24423,7 @@
       <c r="L116" s="10"/>
       <c r="M116" s="10"/>
     </row>
-    <row r="117" spans="1:13" ht="15">
+    <row r="117" spans="1:13" ht="15.75">
       <c r="A117" s="10">
         <v>115</v>
       </c>
@@ -24497,7 +24497,7 @@
       <c r="L118" s="10"/>
       <c r="M118" s="10"/>
     </row>
-    <row r="119" spans="1:13" ht="15">
+    <row r="119" spans="1:13" ht="15.75">
       <c r="A119" s="10">
         <v>117</v>
       </c>
@@ -24534,7 +24534,7 @@
       <c r="L119" s="10"/>
       <c r="M119" s="10"/>
     </row>
-    <row r="120" spans="1:13" ht="15">
+    <row r="120" spans="1:13" ht="15.75">
       <c r="A120" s="10">
         <v>118</v>
       </c>
@@ -24571,7 +24571,7 @@
       <c r="L120" s="10"/>
       <c r="M120" s="10"/>
     </row>
-    <row r="121" spans="1:13" ht="15">
+    <row r="121" spans="1:13" ht="15.75">
       <c r="A121" s="10">
         <v>119</v>
       </c>
@@ -24608,7 +24608,7 @@
       <c r="L121" s="10"/>
       <c r="M121" s="10"/>
     </row>
-    <row r="122" spans="1:13" ht="15">
+    <row r="122" spans="1:13" ht="15.75">
       <c r="A122" s="10">
         <v>120</v>
       </c>
@@ -24645,7 +24645,7 @@
       <c r="L122" s="10"/>
       <c r="M122" s="10"/>
     </row>
-    <row r="123" spans="1:13" ht="15">
+    <row r="123" spans="1:13" ht="15.75">
       <c r="A123" s="10">
         <v>121</v>
       </c>
@@ -24682,7 +24682,7 @@
       <c r="L123" s="10"/>
       <c r="M123" s="10"/>
     </row>
-    <row r="124" spans="1:13" ht="15">
+    <row r="124" spans="1:13" ht="15.75">
       <c r="A124" s="10">
         <v>122</v>
       </c>
@@ -24719,7 +24719,7 @@
       <c r="L124" s="10"/>
       <c r="M124" s="10"/>
     </row>
-    <row r="125" spans="1:13" ht="15">
+    <row r="125" spans="1:13" ht="15.75">
       <c r="A125" s="10">
         <v>123</v>
       </c>
@@ -24756,7 +24756,7 @@
       <c r="L125" s="10"/>
       <c r="M125" s="10"/>
     </row>
-    <row r="126" spans="1:13" ht="15">
+    <row r="126" spans="1:13" ht="15.75">
       <c r="A126" s="10">
         <v>124</v>
       </c>
@@ -24793,7 +24793,7 @@
       <c r="L126" s="10"/>
       <c r="M126" s="10"/>
     </row>
-    <row r="127" spans="1:13" ht="15">
+    <row r="127" spans="1:13" ht="15.75">
       <c r="A127" s="10">
         <v>125</v>
       </c>
@@ -24830,7 +24830,7 @@
       <c r="L127" s="10"/>
       <c r="M127" s="10"/>
     </row>
-    <row r="128" spans="1:13" ht="15">
+    <row r="128" spans="1:13" ht="15.75">
       <c r="A128" s="10">
         <v>126</v>
       </c>
@@ -24867,7 +24867,7 @@
       <c r="L128" s="10"/>
       <c r="M128" s="10"/>
     </row>
-    <row r="129" spans="1:13" ht="15">
+    <row r="129" spans="1:13" ht="15.75">
       <c r="A129" s="10">
         <v>127</v>
       </c>
@@ -24904,7 +24904,7 @@
       <c r="L129" s="10"/>
       <c r="M129" s="10"/>
     </row>
-    <row r="130" spans="1:13" ht="15">
+    <row r="130" spans="1:13" ht="15.75">
       <c r="A130" s="10">
         <v>128</v>
       </c>
@@ -24941,7 +24941,7 @@
       <c r="L130" s="10"/>
       <c r="M130" s="10"/>
     </row>
-    <row r="131" spans="1:13" ht="15">
+    <row r="131" spans="1:13" ht="15.75">
       <c r="A131" s="10">
         <v>129</v>
       </c>
@@ -24980,7 +24980,7 @@
       </c>
       <c r="M131" s="10"/>
     </row>
-    <row r="132" spans="1:13" ht="15">
+    <row r="132" spans="1:13" ht="15.75">
       <c r="A132" s="10">
         <v>130</v>
       </c>
@@ -25017,7 +25017,7 @@
       <c r="L132" s="10"/>
       <c r="M132" s="10"/>
     </row>
-    <row r="133" spans="1:13" ht="15">
+    <row r="133" spans="1:13" ht="15.75">
       <c r="A133" s="10">
         <v>131</v>
       </c>
@@ -25056,7 +25056,7 @@
       </c>
       <c r="M133" s="10"/>
     </row>
-    <row r="134" spans="1:13" ht="15">
+    <row r="134" spans="1:13" ht="15.75">
       <c r="A134" s="10">
         <v>132</v>
       </c>
@@ -25095,7 +25095,7 @@
       </c>
       <c r="M134" s="10"/>
     </row>
-    <row r="135" spans="1:13" ht="15">
+    <row r="135" spans="1:13" ht="15.75">
       <c r="A135" s="10">
         <v>133</v>
       </c>
@@ -25134,7 +25134,7 @@
       </c>
       <c r="M135" s="10"/>
     </row>
-    <row r="136" spans="1:13" ht="15">
+    <row r="136" spans="1:13" ht="15.75">
       <c r="A136" s="10">
         <v>134</v>
       </c>
@@ -25171,7 +25171,7 @@
       <c r="L136" s="10"/>
       <c r="M136" s="10"/>
     </row>
-    <row r="137" spans="1:13" ht="15">
+    <row r="137" spans="1:13" ht="15.75">
       <c r="A137" s="10">
         <v>135</v>
       </c>
@@ -25210,7 +25210,7 @@
       </c>
       <c r="M137" s="10"/>
     </row>
-    <row r="138" spans="1:13" ht="15">
+    <row r="138" spans="1:13" ht="15.75">
       <c r="A138" s="10">
         <v>136</v>
       </c>
@@ -25247,7 +25247,7 @@
       <c r="L138" s="10"/>
       <c r="M138" s="10"/>
     </row>
-    <row r="139" spans="1:13" ht="15">
+    <row r="139" spans="1:13" ht="15.75">
       <c r="A139" s="10">
         <v>137</v>
       </c>
@@ -25286,7 +25286,7 @@
       </c>
       <c r="M139" s="10"/>
     </row>
-    <row r="140" spans="1:13" ht="15">
+    <row r="140" spans="1:13" ht="15.75">
       <c r="A140" s="10">
         <v>138</v>
       </c>
@@ -25325,7 +25325,7 @@
       </c>
       <c r="M140" s="10"/>
     </row>
-    <row r="141" spans="1:13" ht="15">
+    <row r="141" spans="1:13" ht="15.75">
       <c r="A141" s="10">
         <v>139</v>
       </c>
@@ -25364,7 +25364,7 @@
       </c>
       <c r="M141" s="10"/>
     </row>
-    <row r="142" spans="1:13" ht="15">
+    <row r="142" spans="1:13" ht="15.75">
       <c r="A142" s="10">
         <v>140</v>
       </c>
@@ -25403,7 +25403,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="15">
+    <row r="143" spans="1:13" ht="15.75">
       <c r="A143" s="10">
         <v>141</v>
       </c>
@@ -25442,7 +25442,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="15">
+    <row r="144" spans="1:13" ht="15.75">
       <c r="A144" s="10">
         <v>142</v>
       </c>
@@ -25481,7 +25481,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="15">
+    <row r="145" spans="1:13" ht="15.75">
       <c r="A145" s="10">
         <v>143</v>
       </c>
@@ -25518,7 +25518,7 @@
       <c r="L145" s="10"/>
       <c r="M145" s="10"/>
     </row>
-    <row r="146" spans="1:13" ht="15">
+    <row r="146" spans="1:13" ht="15.75">
       <c r="A146" s="10">
         <v>144</v>
       </c>
@@ -25555,7 +25555,7 @@
       <c r="L146" s="10"/>
       <c r="M146" s="10"/>
     </row>
-    <row r="147" spans="1:13" ht="15">
+    <row r="147" spans="1:13" ht="15.75">
       <c r="A147" s="10">
         <v>145</v>
       </c>
@@ -25592,7 +25592,7 @@
       <c r="L147" s="10"/>
       <c r="M147" s="10"/>
     </row>
-    <row r="148" spans="1:13" ht="15">
+    <row r="148" spans="1:13" ht="15.75">
       <c r="A148" s="10">
         <v>146</v>
       </c>
@@ -25629,7 +25629,7 @@
       <c r="L148" s="10"/>
       <c r="M148" s="10"/>
     </row>
-    <row r="149" spans="1:13" ht="15">
+    <row r="149" spans="1:13" ht="15.75">
       <c r="A149" s="10">
         <v>147</v>
       </c>
@@ -25666,7 +25666,7 @@
       <c r="L149" s="10"/>
       <c r="M149" s="10"/>
     </row>
-    <row r="150" spans="1:13" ht="15">
+    <row r="150" spans="1:13" ht="15.75">
       <c r="A150" s="10">
         <v>148</v>
       </c>
@@ -25703,7 +25703,7 @@
       <c r="L150" s="10"/>
       <c r="M150" s="10"/>
     </row>
-    <row r="151" spans="1:13" ht="15">
+    <row r="151" spans="1:13" ht="15.75">
       <c r="A151" s="10">
         <v>149</v>
       </c>
@@ -25740,7 +25740,7 @@
       <c r="L151" s="10"/>
       <c r="M151" s="10"/>
     </row>
-    <row r="152" spans="1:13" ht="15">
+    <row r="152" spans="1:13" ht="15.75">
       <c r="A152" s="10">
         <v>150</v>
       </c>
@@ -25777,7 +25777,7 @@
       <c r="L152" s="10"/>
       <c r="M152" s="10"/>
     </row>
-    <row r="153" spans="1:13" ht="15">
+    <row r="153" spans="1:13" ht="15.75">
       <c r="A153" s="10">
         <v>151</v>
       </c>
@@ -25814,7 +25814,7 @@
       <c r="L153" s="10"/>
       <c r="M153" s="10"/>
     </row>
-    <row r="154" spans="1:13" ht="15">
+    <row r="154" spans="1:13" ht="15.75">
       <c r="A154" s="10">
         <v>152</v>
       </c>
@@ -25851,7 +25851,7 @@
       <c r="L154" s="10"/>
       <c r="M154" s="10"/>
     </row>
-    <row r="155" spans="1:13" ht="15">
+    <row r="155" spans="1:13" ht="15.75">
       <c r="A155" s="10">
         <v>153</v>
       </c>
@@ -25888,7 +25888,7 @@
       <c r="L155" s="10"/>
       <c r="M155" s="10"/>
     </row>
-    <row r="156" spans="1:13" ht="15">
+    <row r="156" spans="1:13" ht="15.75">
       <c r="A156" s="10">
         <v>154</v>
       </c>
@@ -25925,7 +25925,7 @@
       <c r="L156" s="10"/>
       <c r="M156" s="10"/>
     </row>
-    <row r="157" spans="1:13" ht="15">
+    <row r="157" spans="1:13" ht="15.75">
       <c r="A157" s="10">
         <v>155</v>
       </c>
@@ -25962,7 +25962,7 @@
       <c r="L157" s="10"/>
       <c r="M157" s="10"/>
     </row>
-    <row r="158" spans="1:13" ht="15">
+    <row r="158" spans="1:13" ht="15.75">
       <c r="A158" s="10">
         <v>156</v>
       </c>
@@ -25999,7 +25999,7 @@
       <c r="L158" s="10"/>
       <c r="M158" s="10"/>
     </row>
-    <row r="159" spans="1:13" ht="15">
+    <row r="159" spans="1:13" ht="15.75">
       <c r="A159" s="10">
         <v>157</v>
       </c>
@@ -26036,7 +26036,7 @@
       <c r="L159" s="10"/>
       <c r="M159" s="10"/>
     </row>
-    <row r="160" spans="1:13" ht="15">
+    <row r="160" spans="1:13" ht="15.75">
       <c r="A160" s="10">
         <v>158</v>
       </c>
@@ -26073,7 +26073,7 @@
       <c r="L160" s="10"/>
       <c r="M160" s="10"/>
     </row>
-    <row r="161" spans="1:13" ht="15">
+    <row r="161" spans="1:13" ht="15.75">
       <c r="A161" s="10">
         <v>159</v>
       </c>
@@ -26110,7 +26110,7 @@
       <c r="L161" s="10"/>
       <c r="M161" s="10"/>
     </row>
-    <row r="162" spans="1:13" ht="15">
+    <row r="162" spans="1:13" ht="15.75">
       <c r="A162" s="10">
         <v>160</v>
       </c>
@@ -26147,7 +26147,7 @@
       <c r="L162" s="10"/>
       <c r="M162" s="10"/>
     </row>
-    <row r="163" spans="1:13" ht="15">
+    <row r="163" spans="1:13" ht="15.75">
       <c r="A163" s="10">
         <v>161</v>
       </c>
@@ -26184,7 +26184,7 @@
       <c r="L163" s="10"/>
       <c r="M163" s="10"/>
     </row>
-    <row r="164" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="164" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A164" s="10">
         <v>162</v>
       </c>
@@ -26221,7 +26221,7 @@
       <c r="L164" s="10"/>
       <c r="M164" s="10"/>
     </row>
-    <row r="165" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="165" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A165" s="10">
         <v>163</v>
       </c>
@@ -26258,7 +26258,7 @@
       <c r="L165" s="10"/>
       <c r="M165" s="10"/>
     </row>
-    <row r="166" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="166" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A166" s="10">
         <v>164</v>
       </c>
@@ -26295,7 +26295,7 @@
       <c r="L166" s="10"/>
       <c r="M166" s="10"/>
     </row>
-    <row r="167" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="167" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A167" s="10">
         <v>165</v>
       </c>
@@ -26332,7 +26332,7 @@
       <c r="L167" s="10"/>
       <c r="M167" s="10"/>
     </row>
-    <row r="168" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="168" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A168" s="10">
         <v>166</v>
       </c>
@@ -26369,7 +26369,7 @@
       <c r="L168" s="10"/>
       <c r="M168" s="10"/>
     </row>
-    <row r="169" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="169" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A169" s="10">
         <v>167</v>
       </c>
@@ -26406,7 +26406,7 @@
       <c r="L169" s="10"/>
       <c r="M169" s="10"/>
     </row>
-    <row r="170" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="170" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A170" s="10">
         <v>168</v>
       </c>
@@ -26443,7 +26443,7 @@
       <c r="L170" s="10"/>
       <c r="M170" s="10"/>
     </row>
-    <row r="171" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="171" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A171" s="10">
         <v>169</v>
       </c>
@@ -26480,7 +26480,7 @@
       <c r="L171" s="10"/>
       <c r="M171" s="10"/>
     </row>
-    <row r="172" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="172" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A172" s="10">
         <v>170</v>
       </c>
@@ -26517,7 +26517,7 @@
       <c r="L172" s="10"/>
       <c r="M172" s="10"/>
     </row>
-    <row r="173" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="173" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A173" s="10">
         <v>171</v>
       </c>
@@ -26554,7 +26554,7 @@
       <c r="L173" s="10"/>
       <c r="M173" s="10"/>
     </row>
-    <row r="174" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="174" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A174" s="10">
         <v>172</v>
       </c>
@@ -26591,7 +26591,7 @@
       <c r="L174" s="10"/>
       <c r="M174" s="10"/>
     </row>
-    <row r="175" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="175" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A175" s="10">
         <v>173</v>
       </c>
@@ -26628,7 +26628,7 @@
       <c r="L175" s="10"/>
       <c r="M175" s="10"/>
     </row>
-    <row r="176" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="176" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A176" s="10">
         <v>174</v>
       </c>
@@ -26665,7 +26665,7 @@
       <c r="L176" s="10"/>
       <c r="M176" s="10"/>
     </row>
-    <row r="177" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="177" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A177" s="10">
         <v>175</v>
       </c>
@@ -26702,7 +26702,7 @@
       <c r="L177" s="10"/>
       <c r="M177" s="10"/>
     </row>
-    <row r="178" spans="1:13" s="56" customFormat="1" ht="15">
+    <row r="178" spans="1:13" s="56" customFormat="1" ht="15.75">
       <c r="A178" s="10">
         <v>176</v>
       </c>
@@ -26739,7 +26739,7 @@
       <c r="L178" s="10"/>
       <c r="M178" s="10"/>
     </row>
-    <row r="179" spans="1:13" ht="15">
+    <row r="179" spans="1:13" ht="15.75">
       <c r="A179" s="10">
         <v>177</v>
       </c>
@@ -26776,7 +26776,7 @@
       <c r="L179" s="10"/>
       <c r="M179" s="10"/>
     </row>
-    <row r="180" spans="1:13" ht="15">
+    <row r="180" spans="1:13" ht="15.75">
       <c r="A180" s="10">
         <v>178</v>
       </c>
@@ -26813,7 +26813,7 @@
       <c r="L180" s="10"/>
       <c r="M180" s="10"/>
     </row>
-    <row r="181" spans="1:13" ht="15">
+    <row r="181" spans="1:13" ht="15.75">
       <c r="A181" s="10">
         <v>179</v>
       </c>
@@ -26875,15 +26875,15 @@
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="37" customFormat="1" ht="15">
+    <row r="1" spans="1:11" s="37" customFormat="1" ht="15.75">
       <c r="A1" s="37" t="s">
         <v>1294</v>
       </c>
@@ -26918,7 +26918,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="37" customFormat="1" ht="15">
+    <row r="2" spans="1:11" s="37" customFormat="1" ht="15.75">
       <c r="F2" s="6" t="s">
         <v>985</v>
       </c>
@@ -26982,17 +26982,17 @@
       <selection activeCell="G20" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="36" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -29948,19 +29948,19 @@
       <selection activeCell="H24" sqref="A24:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="22.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -31660,7 +31660,7 @@
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
     </row>
-    <row r="50" spans="1:17" ht="28">
+    <row r="50" spans="1:17" ht="45">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -32494,7 +32494,7 @@
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="1:17" ht="28">
+    <row r="80" spans="1:17" ht="45">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -33332,7 +33332,7 @@
       <c r="P104" s="6"/>
       <c r="Q104" s="6"/>
     </row>
-    <row r="105" spans="1:17" ht="28">
+    <row r="105" spans="1:17" ht="30">
       <c r="A105" s="6" t="s">
         <v>215</v>
       </c>
@@ -33377,7 +33377,7 @@
       <c r="P105" s="6"/>
       <c r="Q105" s="6"/>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" ht="30">
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -33399,7 +33399,7 @@
       <c r="P106" s="6"/>
       <c r="Q106" s="6"/>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" ht="30">
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
@@ -34903,7 +34903,7 @@
       <c r="P164" s="6"/>
       <c r="Q164" s="6"/>
     </row>
-    <row r="165" spans="1:17" ht="28">
+    <row r="165" spans="1:17" ht="30">
       <c r="A165" s="6" t="s">
         <v>256</v>
       </c>
@@ -35107,7 +35107,7 @@
       <c r="P171" s="6"/>
       <c r="Q171" s="6"/>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="1:17" ht="30">
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
@@ -38058,17 +38058,17 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="53.5" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -40125,11 +40125,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="52.1640625" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
set sex as subClassOf participant for making it consistent with PRISM project
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@74549 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/amazonia/Amazonia_metadata.xlsx
@@ -8568,8 +8568,8 @@
   <dimension ref="A1:O283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10919,11 +10919,11 @@
       <c r="B60" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>540</v>
+      <c r="C60" s="9" t="s">
+        <v>561</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>541</v>
+        <v>562</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>50</v>

</xml_diff>